<commit_message>
them bang phan cong
</commit_message>
<xml_diff>
--- a/Phân chia công việc.xlsx
+++ b/Phân chia công việc.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26426"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1067E23D-AB85-4B11-AEBD-DA4F335046B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90537C01-B8E4-49AE-B2C7-392C79E89B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>PROJECT DINNER</t>
   </si>
@@ -133,12 +133,15 @@
   <si>
     <t>Link web :https://theviet226.github.io/BC-Capstone_Bootstrap/</t>
   </si>
+  <si>
+    <t>Video review web : https://drive.google.com/file/d/1Xk18Xn1If_x7BIARHl7i8hyHEwjo2ivP/view?usp=sharing</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,8 +221,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +260,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -435,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -503,6 +519,9 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -819,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:G19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1190,7 +1209,7 @@
       </c>
       <c r="H15" s="11"/>
     </row>
-    <row r="17" spans="2:7" ht="25.5" customHeight="1">
+    <row r="17" spans="2:8" ht="25.5" customHeight="1">
       <c r="B17" s="22" t="s">
         <v>25</v>
       </c>
@@ -1200,7 +1219,7 @@
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:8">
       <c r="B18" s="24" t="s">
         <v>26</v>
       </c>
@@ -1210,7 +1229,7 @@
       <c r="F18" s="24"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:8">
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
@@ -1218,11 +1237,32 @@
       <c r="F19" s="24"/>
       <c r="G19" s="24"/>
     </row>
+    <row r="20" spans="2:8" ht="15" customHeight="1">
+      <c r="B20" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+    </row>
+    <row r="21" spans="2:8" ht="15" customHeight="1">
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B18:G19"/>
+    <mergeCell ref="B20:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>